<commit_message>
add/remove user from system. fixed some bugs with add team.
</commit_message>
<xml_diff>
--- a/monster-golf-docs/monster2015/MonsterAll2015.xlsx
+++ b/monster-golf-docs/monster2015/MonsterAll2015.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dsw002002\awald_source\monster-golf\monster-golf-docs\monster2015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\awald\monster-golf\monster-golf-docs\monster2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8985" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Teams" sheetId="1" r:id="rId1"/>
+    <sheet name="Side" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Aaron Wald - Personal View" guid="{0207575D-3FDA-441D-8E09-487CC75706CC}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1616" windowHeight="886" activeSheetId="2"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="163">
   <si>
     <t>Jake</t>
   </si>
@@ -489,6 +493,30 @@
   </si>
   <si>
     <t>LastScored</t>
+  </si>
+  <si>
+    <t>pay spots</t>
+  </si>
+  <si>
+    <t>total purse</t>
+  </si>
+  <si>
+    <t>per team</t>
+  </si>
+  <si>
+    <t>pay per team</t>
+  </si>
+  <si>
+    <t>pay per tier</t>
+  </si>
+  <si>
+    <t>pay % per tier</t>
+  </si>
+  <si>
+    <t>tiered side bet</t>
+  </si>
+  <si>
+    <t># teams</t>
   </si>
 </sst>
 </file>
@@ -496,7 +524,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -539,12 +567,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,6 +597,70 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2C1E74DA-FFD1-41B0-B779-B9130FF11707}" diskRevisions="1" revisionId="3" version="4" preserveHistory="45">
+  <header guid="{8348E4B2-1FB9-4AE6-8955-B629DA260A7E}" dateTime="2015-04-28T11:25:30" maxSheetId="3" userName="Aaron Wald" r:id="rId1">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AB9A472A-6BC6-4B9D-8F6D-6B41995992FF}" dateTime="2015-04-28T11:27:29" maxSheetId="3" userName="Aaron Wald" r:id="rId2" minRId="1">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C2BE5435-E020-4A2E-8535-C069AA757C77}" dateTime="2015-04-28T11:27:51" maxSheetId="3" userName="Aaron Wald" r:id="rId3" minRId="2" maxRId="3">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2C1E74DA-FFD1-41B0-B779-B9130FF11707}" dateTime="2015-04-28T11:30:06" maxSheetId="3" userName="Aaron Wald" r:id="rId4">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="2">
+    <oc r="B2">
+      <v>275</v>
+    </oc>
+    <nc r="B2">
+      <v>100</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rsnm rId="2" sheetId="1" oldName="[MonsterAll2015.xlsx]Sheet1" newName="[MonsterAll2015.xlsx]Teams"/>
+  <rsnm rId="3" sheetId="2" oldName="[MonsterAll2015.xlsx]Sheet2" newName="[MonsterAll2015.xlsx]Side"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{0207575D-3FDA-441D-8E09-487CC75706CC}" action="delete"/>
+  <rcv guid="{0207575D-3FDA-441D-8E09-487CC75706CC}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -827,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -3458,7 +3559,141 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{0207575D-3FDA-441D-8E09-487CC75706CC}">
+      <selection activeCell="G10" sqref="G10"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="6" t="str">
+        <f>(CONCATENATE("pay spots ",$D$2/3))</f>
+        <v>pay spots 4</v>
+      </c>
+      <c r="F1" s="6" t="str">
+        <f t="shared" ref="F1:G1" si="0">(CONCATENATE("pay spots ",$D$2/3))</f>
+        <v>pay spots 4</v>
+      </c>
+      <c r="G1" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>pay spots 4</v>
+      </c>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="8">
+        <v>100</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="6">
+        <f>(3*(_xlfn.FLOOR.MATH(B2/50)-1))+9</f>
+        <v>12</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="9">
+        <v>40</v>
+      </c>
+      <c r="C3" s="7">
+        <f>B3*B2</f>
+        <v>4000</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7">
+        <f>C3*E2</f>
+        <v>2400</v>
+      </c>
+      <c r="F3" s="7">
+        <f>C3*F2</f>
+        <v>1200</v>
+      </c>
+      <c r="G3" s="7">
+        <f>C3*G2</f>
+        <v>400</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7">
+        <f>E3/($D$2/3)</f>
+        <v>600</v>
+      </c>
+      <c r="F4" s="7">
+        <f t="shared" ref="F4:G4" si="1">F3/($D$2/3)</f>
+        <v>300</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{0207575D-3FDA-441D-8E09-487CC75706CC}">
+      <selection activeCell="E4" sqref="E4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>